<commit_message>
changes in get janiza and pqmain
</commit_message>
<xml_diff>
--- a/Janitza-Manual-UMG96RM-Modbus-adress-list.xlsx
+++ b/Janitza-Manual-UMG96RM-Modbus-adress-list.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malte\Documents\GitHub\energy-monitoring\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="204"/>
   </bookViews>
@@ -2996,8 +3001,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -3091,22 +3096,22 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -3119,6 +3124,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3446,23 +3459,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4044"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A1543" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A1547" sqref="A1547"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="3.83203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="2.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="2.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" customHeight="1">
@@ -4149,10 +4162,10 @@
       <c r="D38" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F38" s="3"/>
+      <c r="F38" s="4"/>
       <c r="G38" s="2">
         <v>5</v>
       </c>
@@ -5951,10 +5964,10 @@
       <c r="D163" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E163" s="3" t="s">
+      <c r="E163" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="F163" s="3"/>
+      <c r="F163" s="4"/>
     </row>
     <row r="164" spans="1:7" ht="14.25" customHeight="1">
       <c r="A164" s="2">
@@ -5969,10 +5982,10 @@
       <c r="D164" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E164" s="3" t="s">
+      <c r="E164" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="F164" s="3"/>
+      <c r="F164" s="4"/>
     </row>
     <row r="165" spans="1:7" ht="14.25" customHeight="1">
       <c r="A165" s="2">
@@ -6190,10 +6203,10 @@
       <c r="A175" s="2">
         <v>761</v>
       </c>
-      <c r="B175" s="3" t="s">
+      <c r="B175" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C175" s="3"/>
+      <c r="C175" s="4"/>
       <c r="D175" s="1" t="s">
         <v>10</v>
       </c>
@@ -13905,7 +13918,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="548" spans="1:7" ht="28">
+    <row r="548" spans="1:7" ht="30">
       <c r="A548" s="1">
         <v>3490</v>
       </c>
@@ -16382,10 +16395,10 @@
       <c r="D667" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E667" s="3" t="s">
+      <c r="E667" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="F667" s="3"/>
+      <c r="F667" s="4"/>
     </row>
     <row r="668" spans="1:7" ht="14.25" customHeight="1">
       <c r="A668" s="2">
@@ -17624,10 +17637,10 @@
       <c r="D722" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E722" s="3" t="s">
+      <c r="E722" s="4" t="s">
         <v>456</v>
       </c>
-      <c r="F722" s="3"/>
+      <c r="F722" s="4"/>
     </row>
     <row r="723" spans="1:7" ht="14.25" customHeight="1">
       <c r="A723" s="2">
@@ -17666,7 +17679,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="725" spans="1:7" ht="28">
+    <row r="725" spans="1:7" ht="30">
       <c r="A725" s="1">
         <v>3508</v>
       </c>
@@ -17699,10 +17712,10 @@
       <c r="D726" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E726" s="3" t="s">
+      <c r="E726" s="4" t="s">
         <v>459</v>
       </c>
-      <c r="F726" s="3"/>
+      <c r="F726" s="4"/>
     </row>
     <row r="727" spans="1:7" ht="14.25" customHeight="1">
       <c r="A727" s="2">
@@ -34115,7 +34128,7 @@
     </row>
     <row r="1547" spans="1:7" ht="28.5" customHeight="1">
       <c r="A1547" s="1">
-        <v>1716</v>
+        <v>1714</v>
       </c>
       <c r="B1547" s="1" t="s">
         <v>19</v>
@@ -74097,14 +74110,14 @@
       <c r="B3399" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3399" s="3" t="s">
+      <c r="C3399" s="4" t="s">
         <v>623</v>
       </c>
-      <c r="D3399" s="3"/>
-      <c r="E3399" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3399" s="3"/>
+      <c r="D3399" s="4"/>
+      <c r="E3399" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3399" s="4"/>
     </row>
     <row r="3400" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3400" s="2">
@@ -74113,14 +74126,14 @@
       <c r="B3400" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3400" s="3" t="s">
+      <c r="C3400" s="4" t="s">
         <v>624</v>
       </c>
-      <c r="D3400" s="3"/>
-      <c r="E3400" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3400" s="3"/>
+      <c r="D3400" s="4"/>
+      <c r="E3400" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3400" s="4"/>
     </row>
     <row r="3401" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3401" s="2">
@@ -75203,10 +75216,10 @@
       <c r="C3464" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3464" s="3" t="s">
+      <c r="D3464" s="4" t="s">
         <v>691</v>
       </c>
-      <c r="E3464" s="3"/>
+      <c r="E3464" s="4"/>
       <c r="F3464" s="1" t="s">
         <v>17</v>
       </c>
@@ -75215,10 +75228,10 @@
       </c>
     </row>
     <row r="3465" spans="1:7" ht="14.25" customHeight="1">
-      <c r="D3465" s="3" t="s">
+      <c r="D3465" s="4" t="s">
         <v>692</v>
       </c>
-      <c r="E3465" s="3"/>
+      <c r="E3465" s="4"/>
     </row>
     <row r="3466" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3466" s="2">
@@ -75230,10 +75243,10 @@
       <c r="C3466" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3466" s="3" t="s">
+      <c r="D3466" s="4" t="s">
         <v>693</v>
       </c>
-      <c r="E3466" s="3"/>
+      <c r="E3466" s="4"/>
       <c r="F3466" s="1" t="s">
         <v>17</v>
       </c>
@@ -75242,10 +75255,10 @@
       </c>
     </row>
     <row r="3467" spans="1:7" ht="14.25" customHeight="1">
-      <c r="D3467" s="3" t="s">
+      <c r="D3467" s="4" t="s">
         <v>694</v>
       </c>
-      <c r="E3467" s="3"/>
+      <c r="E3467" s="4"/>
     </row>
     <row r="3468" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3468" s="2">
@@ -75257,10 +75270,10 @@
       <c r="C3468" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3468" s="3" t="s">
+      <c r="D3468" s="4" t="s">
         <v>695</v>
       </c>
-      <c r="E3468" s="3"/>
+      <c r="E3468" s="4"/>
       <c r="F3468" s="1" t="s">
         <v>17</v>
       </c>
@@ -75269,10 +75282,10 @@
       </c>
     </row>
     <row r="3469" spans="1:7" ht="14.25" customHeight="1">
-      <c r="D3469" s="3" t="s">
+      <c r="D3469" s="4" t="s">
         <v>696</v>
       </c>
-      <c r="E3469" s="3"/>
+      <c r="E3469" s="4"/>
     </row>
     <row r="3470" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3470" s="2">
@@ -75284,10 +75297,10 @@
       <c r="C3470" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3470" s="3" t="s">
+      <c r="D3470" s="4" t="s">
         <v>697</v>
       </c>
-      <c r="E3470" s="3"/>
+      <c r="E3470" s="4"/>
       <c r="F3470" s="1" t="s">
         <v>17</v>
       </c>
@@ -75296,10 +75309,10 @@
       </c>
     </row>
     <row r="3471" spans="1:7" ht="14.25" customHeight="1">
-      <c r="D3471" s="3" t="s">
+      <c r="D3471" s="4" t="s">
         <v>698</v>
       </c>
-      <c r="E3471" s="3"/>
+      <c r="E3471" s="4"/>
     </row>
     <row r="3472" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3472" s="2">
@@ -75311,10 +75324,10 @@
       <c r="C3472" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3472" s="3" t="s">
+      <c r="D3472" s="4" t="s">
         <v>699</v>
       </c>
-      <c r="E3472" s="3"/>
+      <c r="E3472" s="4"/>
       <c r="F3472" s="1" t="s">
         <v>17</v>
       </c>
@@ -75332,10 +75345,10 @@
       <c r="C3473" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3473" s="3" t="s">
+      <c r="D3473" s="4" t="s">
         <v>700</v>
       </c>
-      <c r="E3473" s="3"/>
+      <c r="E3473" s="4"/>
       <c r="F3473" s="1" t="s">
         <v>17</v>
       </c>
@@ -75353,10 +75366,10 @@
       <c r="C3474" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3474" s="3" t="s">
+      <c r="D3474" s="4" t="s">
         <v>701</v>
       </c>
-      <c r="E3474" s="3"/>
+      <c r="E3474" s="4"/>
       <c r="F3474" s="1" t="s">
         <v>17</v>
       </c>
@@ -75374,10 +75387,10 @@
       <c r="C3475" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3475" s="3" t="s">
+      <c r="D3475" s="4" t="s">
         <v>702</v>
       </c>
-      <c r="E3475" s="3"/>
+      <c r="E3475" s="4"/>
       <c r="F3475" s="1" t="s">
         <v>17</v>
       </c>
@@ -75395,10 +75408,10 @@
       <c r="C3476" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3476" s="3" t="s">
+      <c r="D3476" s="4" t="s">
         <v>703</v>
       </c>
-      <c r="E3476" s="3"/>
+      <c r="E3476" s="4"/>
       <c r="F3476" s="1" t="s">
         <v>17</v>
       </c>
@@ -75416,10 +75429,10 @@
       <c r="C3477" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3477" s="3" t="s">
+      <c r="D3477" s="4" t="s">
         <v>704</v>
       </c>
-      <c r="E3477" s="3"/>
+      <c r="E3477" s="4"/>
       <c r="F3477" s="1" t="s">
         <v>17</v>
       </c>
@@ -75437,10 +75450,10 @@
       <c r="C3478" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3478" s="3" t="s">
+      <c r="D3478" s="4" t="s">
         <v>705</v>
       </c>
-      <c r="E3478" s="3"/>
+      <c r="E3478" s="4"/>
       <c r="F3478" s="1" t="s">
         <v>17</v>
       </c>
@@ -75458,10 +75471,10 @@
       <c r="C3479" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3479" s="3" t="s">
+      <c r="D3479" s="4" t="s">
         <v>706</v>
       </c>
-      <c r="E3479" s="3"/>
+      <c r="E3479" s="4"/>
       <c r="F3479" s="1" t="s">
         <v>17</v>
       </c>
@@ -75479,10 +75492,10 @@
       <c r="C3480" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3480" s="3" t="s">
+      <c r="D3480" s="4" t="s">
         <v>707</v>
       </c>
-      <c r="E3480" s="3"/>
+      <c r="E3480" s="4"/>
       <c r="F3480" s="1" t="s">
         <v>17</v>
       </c>
@@ -75500,10 +75513,10 @@
       <c r="C3481" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3481" s="3" t="s">
+      <c r="D3481" s="4" t="s">
         <v>708</v>
       </c>
-      <c r="E3481" s="3"/>
+      <c r="E3481" s="4"/>
       <c r="F3481" s="1" t="s">
         <v>17</v>
       </c>
@@ -75521,10 +75534,10 @@
       <c r="C3482" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3482" s="3" t="s">
+      <c r="D3482" s="4" t="s">
         <v>709</v>
       </c>
-      <c r="E3482" s="3"/>
+      <c r="E3482" s="4"/>
       <c r="F3482" s="1" t="s">
         <v>17</v>
       </c>
@@ -75542,10 +75555,10 @@
       <c r="C3483" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3483" s="3" t="s">
+      <c r="D3483" s="4" t="s">
         <v>710</v>
       </c>
-      <c r="E3483" s="3"/>
+      <c r="E3483" s="4"/>
       <c r="F3483" s="1" t="s">
         <v>17</v>
       </c>
@@ -75563,10 +75576,10 @@
       <c r="C3484" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D3484" s="3" t="s">
+      <c r="D3484" s="4" t="s">
         <v>711</v>
       </c>
-      <c r="E3484" s="3"/>
+      <c r="E3484" s="4"/>
       <c r="F3484" s="1" t="s">
         <v>10</v>
       </c>
@@ -75578,14 +75591,14 @@
       <c r="A3485" s="2">
         <v>25011</v>
       </c>
-      <c r="B3485" s="3" t="s">
+      <c r="B3485" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C3485" s="3"/>
-      <c r="D3485" s="3" t="s">
+      <c r="C3485" s="4"/>
+      <c r="D3485" s="4" t="s">
         <v>712</v>
       </c>
-      <c r="E3485" s="3"/>
+      <c r="E3485" s="4"/>
       <c r="F3485" s="1" t="s">
         <v>10</v>
       </c>
@@ -75603,10 +75616,10 @@
       <c r="C3486" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D3486" s="3" t="s">
+      <c r="D3486" s="4" t="s">
         <v>714</v>
       </c>
-      <c r="E3486" s="3"/>
+      <c r="E3486" s="4"/>
       <c r="F3486" s="1" t="s">
         <v>10</v>
       </c>
@@ -75624,10 +75637,10 @@
       <c r="C3487" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E3487" s="3" t="s">
+      <c r="E3487" s="4" t="s">
         <v>715</v>
       </c>
-      <c r="F3487" s="3"/>
+      <c r="F3487" s="4"/>
     </row>
     <row r="3488" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3488" s="2">
@@ -75639,10 +75652,10 @@
       <c r="C3488" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E3488" s="3" t="s">
+      <c r="E3488" s="4" t="s">
         <v>716</v>
       </c>
-      <c r="F3488" s="3"/>
+      <c r="F3488" s="4"/>
     </row>
     <row r="3489" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3489" s="2">
@@ -75654,10 +75667,10 @@
       <c r="C3489" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E3489" s="3" t="s">
+      <c r="E3489" s="4" t="s">
         <v>717</v>
       </c>
-      <c r="F3489" s="3"/>
+      <c r="F3489" s="4"/>
     </row>
     <row r="3490" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3490" s="2">
@@ -75669,10 +75682,10 @@
       <c r="C3490" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E3490" s="3" t="s">
+      <c r="E3490" s="4" t="s">
         <v>718</v>
       </c>
-      <c r="F3490" s="3"/>
+      <c r="F3490" s="4"/>
     </row>
     <row r="3491" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3491" s="2">
@@ -75684,10 +75697,10 @@
       <c r="C3491" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E3491" s="3" t="s">
+      <c r="E3491" s="4" t="s">
         <v>719</v>
       </c>
-      <c r="F3491" s="3"/>
+      <c r="F3491" s="4"/>
     </row>
     <row r="3492" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3492" s="2">
@@ -75699,10 +75712,10 @@
       <c r="C3492" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E3492" s="3" t="s">
+      <c r="E3492" s="4" t="s">
         <v>720</v>
       </c>
-      <c r="F3492" s="3"/>
+      <c r="F3492" s="4"/>
     </row>
     <row r="3493" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3493" s="2">
@@ -75714,10 +75727,10 @@
       <c r="C3493" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E3493" s="3" t="s">
+      <c r="E3493" s="4" t="s">
         <v>721</v>
       </c>
-      <c r="F3493" s="3"/>
+      <c r="F3493" s="4"/>
     </row>
     <row r="3494" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3494" s="2">
@@ -75729,10 +75742,10 @@
       <c r="C3494" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E3494" s="3" t="s">
+      <c r="E3494" s="4" t="s">
         <v>722</v>
       </c>
-      <c r="F3494" s="3"/>
+      <c r="F3494" s="4"/>
     </row>
     <row r="3495" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3495" s="2">
@@ -75744,10 +75757,10 @@
       <c r="C3495" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E3495" s="3" t="s">
+      <c r="E3495" s="4" t="s">
         <v>723</v>
       </c>
-      <c r="F3495" s="3"/>
+      <c r="F3495" s="4"/>
     </row>
     <row r="3496" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3496" s="2">
@@ -75759,10 +75772,10 @@
       <c r="C3496" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E3496" s="3" t="s">
+      <c r="E3496" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="F3496" s="3"/>
+      <c r="F3496" s="4"/>
     </row>
     <row r="3497" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3497" s="2">
@@ -75774,10 +75787,10 @@
       <c r="C3497" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E3497" s="3" t="s">
+      <c r="E3497" s="4" t="s">
         <v>725</v>
       </c>
-      <c r="F3497" s="3"/>
+      <c r="F3497" s="4"/>
     </row>
     <row r="3498" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3498" s="2">
@@ -75789,10 +75802,10 @@
       <c r="C3498" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E3498" s="3" t="s">
+      <c r="E3498" s="4" t="s">
         <v>726</v>
       </c>
-      <c r="F3498" s="3"/>
+      <c r="F3498" s="4"/>
     </row>
     <row r="3499" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3499" s="2">
@@ -75886,193 +75899,193 @@
       <c r="A3507" s="2">
         <v>10154</v>
       </c>
-      <c r="B3507" s="3" t="s">
+      <c r="B3507" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="C3507" s="3"/>
+      <c r="C3507" s="4"/>
       <c r="D3507" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3507" s="3" t="s">
+      <c r="E3507" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="F3507" s="3"/>
+      <c r="F3507" s="4"/>
     </row>
     <row r="3508" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3508" s="2">
         <v>10156</v>
       </c>
-      <c r="B3508" s="3" t="s">
+      <c r="B3508" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="C3508" s="3"/>
+      <c r="C3508" s="4"/>
       <c r="D3508" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3508" s="3" t="s">
+      <c r="E3508" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="F3508" s="3"/>
+      <c r="F3508" s="4"/>
     </row>
     <row r="3509" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3509" s="2">
         <v>10158</v>
       </c>
-      <c r="B3509" s="3" t="s">
+      <c r="B3509" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="C3509" s="3"/>
+      <c r="C3509" s="4"/>
       <c r="D3509" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3509" s="3" t="s">
+      <c r="E3509" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="F3509" s="3"/>
+      <c r="F3509" s="4"/>
     </row>
     <row r="3510" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3510" s="2">
         <v>10160</v>
       </c>
-      <c r="B3510" s="3" t="s">
+      <c r="B3510" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="C3510" s="3"/>
+      <c r="C3510" s="4"/>
       <c r="D3510" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3510" s="3" t="s">
+      <c r="E3510" s="4" t="s">
         <v>736</v>
       </c>
-      <c r="F3510" s="3"/>
+      <c r="F3510" s="4"/>
     </row>
     <row r="3511" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3511" s="2">
         <v>10162</v>
       </c>
-      <c r="B3511" s="3" t="s">
+      <c r="B3511" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="C3511" s="3"/>
+      <c r="C3511" s="4"/>
       <c r="D3511" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3511" s="3" t="s">
+      <c r="E3511" s="4" t="s">
         <v>737</v>
       </c>
-      <c r="F3511" s="3"/>
+      <c r="F3511" s="4"/>
     </row>
     <row r="3512" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3512" s="2">
         <v>10164</v>
       </c>
-      <c r="B3512" s="3" t="s">
+      <c r="B3512" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="C3512" s="3"/>
+      <c r="C3512" s="4"/>
       <c r="D3512" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3512" s="3" t="s">
+      <c r="E3512" s="4" t="s">
         <v>738</v>
       </c>
-      <c r="F3512" s="3"/>
+      <c r="F3512" s="4"/>
     </row>
     <row r="3513" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3513" s="2">
         <v>10166</v>
       </c>
-      <c r="B3513" s="3" t="s">
+      <c r="B3513" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="C3513" s="3"/>
+      <c r="C3513" s="4"/>
       <c r="D3513" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3513" s="3" t="s">
+      <c r="E3513" s="4" t="s">
         <v>739</v>
       </c>
-      <c r="F3513" s="3"/>
+      <c r="F3513" s="4"/>
     </row>
     <row r="3514" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3514" s="2">
         <v>10168</v>
       </c>
-      <c r="B3514" s="3" t="s">
+      <c r="B3514" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="C3514" s="3"/>
+      <c r="C3514" s="4"/>
       <c r="D3514" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3514" s="3" t="s">
+      <c r="E3514" s="4" t="s">
         <v>740</v>
       </c>
-      <c r="F3514" s="3"/>
+      <c r="F3514" s="4"/>
     </row>
     <row r="3515" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3515" s="2">
         <v>10170</v>
       </c>
-      <c r="B3515" s="3" t="s">
+      <c r="B3515" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="C3515" s="3"/>
+      <c r="C3515" s="4"/>
       <c r="D3515" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3515" s="3" t="s">
+      <c r="E3515" s="4" t="s">
         <v>741</v>
       </c>
-      <c r="F3515" s="3"/>
+      <c r="F3515" s="4"/>
     </row>
     <row r="3516" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3516" s="2">
         <v>10172</v>
       </c>
-      <c r="B3516" s="3" t="s">
+      <c r="B3516" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="C3516" s="3"/>
+      <c r="C3516" s="4"/>
       <c r="D3516" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3516" s="3" t="s">
+      <c r="E3516" s="4" t="s">
         <v>742</v>
       </c>
-      <c r="F3516" s="3"/>
+      <c r="F3516" s="4"/>
     </row>
     <row r="3517" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3517" s="2">
         <v>10174</v>
       </c>
-      <c r="B3517" s="3" t="s">
+      <c r="B3517" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="C3517" s="3"/>
+      <c r="C3517" s="4"/>
       <c r="D3517" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3517" s="3" t="s">
+      <c r="E3517" s="4" t="s">
         <v>743</v>
       </c>
-      <c r="F3517" s="3"/>
+      <c r="F3517" s="4"/>
     </row>
     <row r="3518" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3518" s="2">
         <v>10176</v>
       </c>
-      <c r="B3518" s="3" t="s">
+      <c r="B3518" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="C3518" s="3"/>
+      <c r="C3518" s="4"/>
       <c r="D3518" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3518" s="3" t="s">
+      <c r="E3518" s="4" t="s">
         <v>744</v>
       </c>
-      <c r="F3518" s="3"/>
+      <c r="F3518" s="4"/>
     </row>
     <row r="3519" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3519" s="2">
@@ -76087,10 +76100,10 @@
       <c r="D3519" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3519" s="3" t="s">
+      <c r="E3519" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="F3519" s="3"/>
+      <c r="F3519" s="4"/>
     </row>
     <row r="3520" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3520" s="2">
@@ -76105,10 +76118,10 @@
       <c r="D3520" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3520" s="3" t="s">
+      <c r="E3520" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="F3520" s="3"/>
+      <c r="F3520" s="4"/>
     </row>
     <row r="3521" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3521" s="2">
@@ -76123,10 +76136,10 @@
       <c r="D3521" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3521" s="3" t="s">
+      <c r="E3521" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="F3521" s="3"/>
+      <c r="F3521" s="4"/>
     </row>
     <row r="3522" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3522" s="2">
@@ -76141,10 +76154,10 @@
       <c r="D3522" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3522" s="3" t="s">
+      <c r="E3522" s="4" t="s">
         <v>736</v>
       </c>
-      <c r="F3522" s="3"/>
+      <c r="F3522" s="4"/>
     </row>
     <row r="3523" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3523" s="2">
@@ -76159,10 +76172,10 @@
       <c r="D3523" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3523" s="3" t="s">
+      <c r="E3523" s="4" t="s">
         <v>737</v>
       </c>
-      <c r="F3523" s="3"/>
+      <c r="F3523" s="4"/>
     </row>
     <row r="3524" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3524" s="2">
@@ -76177,10 +76190,10 @@
       <c r="D3524" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3524" s="3" t="s">
+      <c r="E3524" s="4" t="s">
         <v>738</v>
       </c>
-      <c r="F3524" s="3"/>
+      <c r="F3524" s="4"/>
     </row>
     <row r="3525" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3525" s="2">
@@ -76195,10 +76208,10 @@
       <c r="D3525" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3525" s="3" t="s">
+      <c r="E3525" s="4" t="s">
         <v>739</v>
       </c>
-      <c r="F3525" s="3"/>
+      <c r="F3525" s="4"/>
     </row>
     <row r="3526" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3526" s="2">
@@ -76213,10 +76226,10 @@
       <c r="D3526" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3526" s="3" t="s">
+      <c r="E3526" s="4" t="s">
         <v>740</v>
       </c>
-      <c r="F3526" s="3"/>
+      <c r="F3526" s="4"/>
     </row>
     <row r="3527" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3527" s="2">
@@ -76231,10 +76244,10 @@
       <c r="D3527" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3527" s="3" t="s">
+      <c r="E3527" s="4" t="s">
         <v>741</v>
       </c>
-      <c r="F3527" s="3"/>
+      <c r="F3527" s="4"/>
     </row>
     <row r="3528" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3528" s="2">
@@ -76249,10 +76262,10 @@
       <c r="D3528" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3528" s="3" t="s">
+      <c r="E3528" s="4" t="s">
         <v>742</v>
       </c>
-      <c r="F3528" s="3"/>
+      <c r="F3528" s="4"/>
     </row>
     <row r="3529" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3529" s="2">
@@ -76267,10 +76280,10 @@
       <c r="D3529" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3529" s="3" t="s">
+      <c r="E3529" s="4" t="s">
         <v>743</v>
       </c>
-      <c r="F3529" s="3"/>
+      <c r="F3529" s="4"/>
     </row>
     <row r="3530" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3530" s="2">
@@ -76285,10 +76298,10 @@
       <c r="D3530" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E3530" s="3" t="s">
+      <c r="E3530" s="4" t="s">
         <v>744</v>
       </c>
-      <c r="F3530" s="3"/>
+      <c r="F3530" s="4"/>
     </row>
     <row r="3531" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3531" s="2">
@@ -76600,10 +76613,10 @@
       <c r="C3549" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3549" s="3" t="s">
+      <c r="D3549" s="4" t="s">
         <v>761</v>
       </c>
-      <c r="E3549" s="3"/>
+      <c r="E3549" s="4"/>
       <c r="F3549" s="1" t="s">
         <v>71</v>
       </c>
@@ -76621,10 +76634,10 @@
       <c r="C3550" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3550" s="3" t="s">
+      <c r="D3550" s="4" t="s">
         <v>762</v>
       </c>
-      <c r="E3550" s="3"/>
+      <c r="E3550" s="4"/>
       <c r="F3550" s="1" t="s">
         <v>81</v>
       </c>
@@ -76642,10 +76655,10 @@
       <c r="C3551" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3551" s="3" t="s">
+      <c r="D3551" s="4" t="s">
         <v>763</v>
       </c>
-      <c r="E3551" s="3"/>
+      <c r="E3551" s="4"/>
       <c r="F3551" s="1" t="s">
         <v>81</v>
       </c>
@@ -76654,10 +76667,10 @@
       </c>
     </row>
     <row r="3552" spans="1:7" ht="14.25" customHeight="1">
-      <c r="D3552" s="3" t="s">
+      <c r="D3552" s="4" t="s">
         <v>746</v>
       </c>
-      <c r="E3552" s="3"/>
+      <c r="E3552" s="4"/>
     </row>
     <row r="3553" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3553" s="2">
@@ -76669,10 +76682,10 @@
       <c r="C3553" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3553" s="3" t="s">
+      <c r="D3553" s="4" t="s">
         <v>764</v>
       </c>
-      <c r="E3553" s="3"/>
+      <c r="E3553" s="4"/>
       <c r="F3553" s="1" t="s">
         <v>85</v>
       </c>
@@ -76690,10 +76703,10 @@
       <c r="C3554" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3554" s="3" t="s">
+      <c r="D3554" s="4" t="s">
         <v>765</v>
       </c>
-      <c r="E3554" s="3"/>
+      <c r="E3554" s="4"/>
       <c r="F3554" s="1" t="s">
         <v>71</v>
       </c>
@@ -76702,10 +76715,10 @@
       </c>
     </row>
     <row r="3555" spans="1:7" ht="14.25" customHeight="1">
-      <c r="D3555" s="3" t="s">
+      <c r="D3555" s="4" t="s">
         <v>749</v>
       </c>
-      <c r="E3555" s="3"/>
+      <c r="E3555" s="4"/>
     </row>
     <row r="3556" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3556" s="2">
@@ -76717,10 +76730,10 @@
       <c r="C3556" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3556" s="3" t="s">
+      <c r="D3556" s="4" t="s">
         <v>766</v>
       </c>
-      <c r="E3556" s="3"/>
+      <c r="E3556" s="4"/>
       <c r="F3556" s="1" t="s">
         <v>71</v>
       </c>
@@ -76738,10 +76751,10 @@
       <c r="C3557" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3557" s="3" t="s">
+      <c r="D3557" s="4" t="s">
         <v>767</v>
       </c>
-      <c r="E3557" s="3"/>
+      <c r="E3557" s="4"/>
       <c r="F3557" s="1" t="s">
         <v>71</v>
       </c>
@@ -76759,10 +76772,10 @@
       <c r="C3558" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3558" s="3" t="s">
+      <c r="D3558" s="4" t="s">
         <v>768</v>
       </c>
-      <c r="E3558" s="3"/>
+      <c r="E3558" s="4"/>
       <c r="F3558" s="1" t="s">
         <v>81</v>
       </c>
@@ -76780,10 +76793,10 @@
       <c r="C3559" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3559" s="3" t="s">
+      <c r="D3559" s="4" t="s">
         <v>769</v>
       </c>
-      <c r="E3559" s="3"/>
+      <c r="E3559" s="4"/>
       <c r="F3559" s="1" t="s">
         <v>85</v>
       </c>
@@ -76801,10 +76814,10 @@
       <c r="C3560" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3560" s="3" t="s">
+      <c r="D3560" s="4" t="s">
         <v>770</v>
       </c>
-      <c r="E3560" s="3"/>
+      <c r="E3560" s="4"/>
       <c r="F3560" s="1" t="s">
         <v>71</v>
       </c>
@@ -76813,10 +76826,10 @@
       </c>
     </row>
     <row r="3561" spans="1:7" ht="14.25" customHeight="1">
-      <c r="D3561" s="3" t="s">
+      <c r="D3561" s="4" t="s">
         <v>749</v>
       </c>
-      <c r="E3561" s="3"/>
+      <c r="E3561" s="4"/>
     </row>
     <row r="3562" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3562" s="2">
@@ -76828,10 +76841,10 @@
       <c r="C3562" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3562" s="3" t="s">
+      <c r="D3562" s="4" t="s">
         <v>771</v>
       </c>
-      <c r="E3562" s="3"/>
+      <c r="E3562" s="4"/>
       <c r="F3562" s="1" t="s">
         <v>71</v>
       </c>
@@ -76849,10 +76862,10 @@
       <c r="C3563" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3563" s="3" t="s">
+      <c r="D3563" s="4" t="s">
         <v>772</v>
       </c>
-      <c r="E3563" s="3"/>
+      <c r="E3563" s="4"/>
       <c r="F3563" s="1" t="s">
         <v>71</v>
       </c>
@@ -76870,10 +76883,10 @@
       <c r="C3564" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3564" s="3" t="s">
+      <c r="D3564" s="4" t="s">
         <v>773</v>
       </c>
-      <c r="E3564" s="3"/>
+      <c r="E3564" s="4"/>
       <c r="F3564" s="1" t="s">
         <v>81</v>
       </c>
@@ -76891,10 +76904,10 @@
       <c r="C3565" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3565" s="3" t="s">
+      <c r="D3565" s="4" t="s">
         <v>774</v>
       </c>
-      <c r="E3565" s="3"/>
+      <c r="E3565" s="4"/>
       <c r="F3565" s="1" t="s">
         <v>85</v>
       </c>
@@ -76912,10 +76925,10 @@
       <c r="C3566" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3566" s="3" t="s">
+      <c r="D3566" s="4" t="s">
         <v>775</v>
       </c>
-      <c r="E3566" s="3"/>
+      <c r="E3566" s="4"/>
       <c r="F3566" s="1" t="s">
         <v>71</v>
       </c>
@@ -76924,10 +76937,10 @@
       </c>
     </row>
     <row r="3567" spans="1:7" ht="14.25" customHeight="1">
-      <c r="D3567" s="3" t="s">
+      <c r="D3567" s="4" t="s">
         <v>749</v>
       </c>
-      <c r="E3567" s="3"/>
+      <c r="E3567" s="4"/>
     </row>
     <row r="3568" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3568" s="2">
@@ -76939,10 +76952,10 @@
       <c r="C3568" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3568" s="3" t="s">
+      <c r="D3568" s="4" t="s">
         <v>776</v>
       </c>
-      <c r="E3568" s="3"/>
+      <c r="E3568" s="4"/>
       <c r="F3568" s="1" t="s">
         <v>71</v>
       </c>
@@ -76960,10 +76973,10 @@
       <c r="C3569" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3569" s="3" t="s">
+      <c r="D3569" s="4" t="s">
         <v>777</v>
       </c>
-      <c r="E3569" s="3"/>
+      <c r="E3569" s="4"/>
       <c r="F3569" s="1" t="s">
         <v>71</v>
       </c>
@@ -76981,10 +76994,10 @@
       <c r="C3570" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3570" s="3" t="s">
+      <c r="D3570" s="4" t="s">
         <v>778</v>
       </c>
-      <c r="E3570" s="3"/>
+      <c r="E3570" s="4"/>
       <c r="F3570" s="1" t="s">
         <v>81</v>
       </c>
@@ -77002,10 +77015,10 @@
       <c r="C3571" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3571" s="3" t="s">
+      <c r="D3571" s="4" t="s">
         <v>779</v>
       </c>
-      <c r="E3571" s="3"/>
+      <c r="E3571" s="4"/>
       <c r="F3571" s="1" t="s">
         <v>81</v>
       </c>
@@ -77014,10 +77027,10 @@
       </c>
     </row>
     <row r="3572" spans="1:7" ht="14.25" customHeight="1">
-      <c r="D3572" s="3" t="s">
+      <c r="D3572" s="4" t="s">
         <v>746</v>
       </c>
-      <c r="E3572" s="3"/>
+      <c r="E3572" s="4"/>
     </row>
     <row r="3573" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3573" s="2">
@@ -77029,10 +77042,10 @@
       <c r="C3573" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3573" s="3" t="s">
+      <c r="D3573" s="4" t="s">
         <v>780</v>
       </c>
-      <c r="E3573" s="3"/>
+      <c r="E3573" s="4"/>
       <c r="F3573" s="1" t="s">
         <v>85</v>
       </c>
@@ -77050,10 +77063,10 @@
       <c r="C3574" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3574" s="3" t="s">
+      <c r="D3574" s="4" t="s">
         <v>781</v>
       </c>
-      <c r="E3574" s="3"/>
+      <c r="E3574" s="4"/>
       <c r="F3574" s="1" t="s">
         <v>71</v>
       </c>
@@ -77062,10 +77075,10 @@
       </c>
     </row>
     <row r="3575" spans="1:7" ht="14.25" customHeight="1">
-      <c r="D3575" s="3" t="s">
+      <c r="D3575" s="4" t="s">
         <v>749</v>
       </c>
-      <c r="E3575" s="3"/>
+      <c r="E3575" s="4"/>
     </row>
     <row r="3576" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3576" s="2">
@@ -77077,10 +77090,10 @@
       <c r="C3576" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3576" s="3" t="s">
+      <c r="D3576" s="4" t="s">
         <v>782</v>
       </c>
-      <c r="E3576" s="3"/>
+      <c r="E3576" s="4"/>
       <c r="F3576" s="1" t="s">
         <v>71</v>
       </c>
@@ -77098,10 +77111,10 @@
       <c r="C3577" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3577" s="3" t="s">
+      <c r="D3577" s="4" t="s">
         <v>783</v>
       </c>
-      <c r="E3577" s="3"/>
+      <c r="E3577" s="4"/>
       <c r="F3577" s="1" t="s">
         <v>71</v>
       </c>
@@ -77119,10 +77132,10 @@
       <c r="C3578" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3578" s="3" t="s">
+      <c r="D3578" s="4" t="s">
         <v>784</v>
       </c>
-      <c r="E3578" s="3"/>
+      <c r="E3578" s="4"/>
       <c r="F3578" s="1" t="s">
         <v>81</v>
       </c>
@@ -77140,10 +77153,10 @@
       <c r="C3579" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3579" s="3" t="s">
+      <c r="D3579" s="4" t="s">
         <v>785</v>
       </c>
-      <c r="E3579" s="3"/>
+      <c r="E3579" s="4"/>
       <c r="F3579" s="1" t="s">
         <v>85</v>
       </c>
@@ -77161,10 +77174,10 @@
       <c r="C3580" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3580" s="3" t="s">
+      <c r="D3580" s="4" t="s">
         <v>786</v>
       </c>
-      <c r="E3580" s="3"/>
+      <c r="E3580" s="4"/>
       <c r="F3580" s="1" t="s">
         <v>71</v>
       </c>
@@ -77173,10 +77186,10 @@
       </c>
     </row>
     <row r="3581" spans="1:7" ht="14.25" customHeight="1">
-      <c r="D3581" s="3" t="s">
+      <c r="D3581" s="4" t="s">
         <v>749</v>
       </c>
-      <c r="E3581" s="3"/>
+      <c r="E3581" s="4"/>
     </row>
     <row r="3582" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3582" s="2">
@@ -77188,10 +77201,10 @@
       <c r="C3582" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3582" s="3" t="s">
+      <c r="D3582" s="4" t="s">
         <v>787</v>
       </c>
-      <c r="E3582" s="3"/>
+      <c r="E3582" s="4"/>
       <c r="F3582" s="1" t="s">
         <v>71</v>
       </c>
@@ -77209,10 +77222,10 @@
       <c r="C3583" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3583" s="3" t="s">
+      <c r="D3583" s="4" t="s">
         <v>788</v>
       </c>
-      <c r="E3583" s="3"/>
+      <c r="E3583" s="4"/>
       <c r="F3583" s="1" t="s">
         <v>71</v>
       </c>
@@ -77230,10 +77243,10 @@
       <c r="C3584" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3584" s="3" t="s">
+      <c r="D3584" s="4" t="s">
         <v>789</v>
       </c>
-      <c r="E3584" s="3"/>
+      <c r="E3584" s="4"/>
       <c r="F3584" s="1" t="s">
         <v>81</v>
       </c>
@@ -77251,10 +77264,10 @@
       <c r="C3585" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3585" s="3" t="s">
+      <c r="D3585" s="4" t="s">
         <v>790</v>
       </c>
-      <c r="E3585" s="3"/>
+      <c r="E3585" s="4"/>
       <c r="F3585" s="1" t="s">
         <v>85</v>
       </c>
@@ -77272,10 +77285,10 @@
       <c r="C3586" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3586" s="3" t="s">
+      <c r="D3586" s="4" t="s">
         <v>791</v>
       </c>
-      <c r="E3586" s="3"/>
+      <c r="E3586" s="4"/>
       <c r="F3586" s="1" t="s">
         <v>71</v>
       </c>
@@ -77284,10 +77297,10 @@
       </c>
     </row>
     <row r="3587" spans="1:7" ht="14.25" customHeight="1">
-      <c r="D3587" s="3" t="s">
+      <c r="D3587" s="4" t="s">
         <v>749</v>
       </c>
-      <c r="E3587" s="3"/>
+      <c r="E3587" s="4"/>
     </row>
     <row r="3588" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3588" s="2">
@@ -77299,10 +77312,10 @@
       <c r="C3588" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3588" s="3" t="s">
+      <c r="D3588" s="4" t="s">
         <v>792</v>
       </c>
-      <c r="E3588" s="3"/>
+      <c r="E3588" s="4"/>
       <c r="F3588" s="1" t="s">
         <v>71</v>
       </c>
@@ -77320,10 +77333,10 @@
       <c r="C3589" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3589" s="3" t="s">
+      <c r="D3589" s="4" t="s">
         <v>793</v>
       </c>
-      <c r="E3589" s="3"/>
+      <c r="E3589" s="4"/>
       <c r="F3589" s="1" t="s">
         <v>71</v>
       </c>
@@ -77341,10 +77354,10 @@
       <c r="C3590" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3590" s="3" t="s">
+      <c r="D3590" s="4" t="s">
         <v>794</v>
       </c>
-      <c r="E3590" s="3"/>
+      <c r="E3590" s="4"/>
       <c r="F3590" s="1" t="s">
         <v>81</v>
       </c>
@@ -77362,10 +77375,10 @@
       <c r="C3591" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3591" s="3" t="s">
+      <c r="D3591" s="4" t="s">
         <v>795</v>
       </c>
-      <c r="E3591" s="3"/>
+      <c r="E3591" s="4"/>
       <c r="F3591" s="1" t="s">
         <v>81</v>
       </c>
@@ -77374,10 +77387,10 @@
       </c>
     </row>
     <row r="3592" spans="1:7" ht="14.25" customHeight="1">
-      <c r="D3592" s="3" t="s">
+      <c r="D3592" s="4" t="s">
         <v>746</v>
       </c>
-      <c r="E3592" s="3"/>
+      <c r="E3592" s="4"/>
     </row>
     <row r="3593" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3593" s="2">
@@ -77389,10 +77402,10 @@
       <c r="C3593" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3593" s="3" t="s">
+      <c r="D3593" s="4" t="s">
         <v>796</v>
       </c>
-      <c r="E3593" s="3"/>
+      <c r="E3593" s="4"/>
       <c r="F3593" s="1" t="s">
         <v>85</v>
       </c>
@@ -77410,10 +77423,10 @@
       <c r="C3594" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3594" s="3" t="s">
+      <c r="D3594" s="4" t="s">
         <v>797</v>
       </c>
-      <c r="E3594" s="3"/>
+      <c r="E3594" s="4"/>
       <c r="F3594" s="1" t="s">
         <v>71</v>
       </c>
@@ -77422,10 +77435,10 @@
       </c>
     </row>
     <row r="3595" spans="1:7" ht="14.25" customHeight="1">
-      <c r="D3595" s="3" t="s">
+      <c r="D3595" s="4" t="s">
         <v>749</v>
       </c>
-      <c r="E3595" s="3"/>
+      <c r="E3595" s="4"/>
     </row>
     <row r="3596" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3596" s="2">
@@ -77437,10 +77450,10 @@
       <c r="C3596" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3596" s="3" t="s">
+      <c r="D3596" s="4" t="s">
         <v>798</v>
       </c>
-      <c r="E3596" s="3"/>
+      <c r="E3596" s="4"/>
       <c r="F3596" s="1" t="s">
         <v>71</v>
       </c>
@@ -77458,10 +77471,10 @@
       <c r="C3597" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3597" s="3" t="s">
+      <c r="D3597" s="4" t="s">
         <v>799</v>
       </c>
-      <c r="E3597" s="3"/>
+      <c r="E3597" s="4"/>
       <c r="F3597" s="1" t="s">
         <v>71</v>
       </c>
@@ -77479,10 +77492,10 @@
       <c r="C3598" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3598" s="3" t="s">
+      <c r="D3598" s="4" t="s">
         <v>800</v>
       </c>
-      <c r="E3598" s="3"/>
+      <c r="E3598" s="4"/>
       <c r="F3598" s="1" t="s">
         <v>81</v>
       </c>
@@ -77500,10 +77513,10 @@
       <c r="C3599" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3599" s="3" t="s">
+      <c r="D3599" s="4" t="s">
         <v>801</v>
       </c>
-      <c r="E3599" s="3"/>
+      <c r="E3599" s="4"/>
       <c r="F3599" s="1" t="s">
         <v>85</v>
       </c>
@@ -77521,10 +77534,10 @@
       <c r="C3600" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3600" s="3" t="s">
+      <c r="D3600" s="4" t="s">
         <v>802</v>
       </c>
-      <c r="E3600" s="3"/>
+      <c r="E3600" s="4"/>
       <c r="F3600" s="1" t="s">
         <v>71</v>
       </c>
@@ -77533,10 +77546,10 @@
       </c>
     </row>
     <row r="3601" spans="1:7" ht="14.25" customHeight="1">
-      <c r="D3601" s="3" t="s">
+      <c r="D3601" s="4" t="s">
         <v>749</v>
       </c>
-      <c r="E3601" s="3"/>
+      <c r="E3601" s="4"/>
     </row>
     <row r="3602" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3602" s="2">
@@ -77548,10 +77561,10 @@
       <c r="C3602" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3602" s="3" t="s">
+      <c r="D3602" s="4" t="s">
         <v>803</v>
       </c>
-      <c r="E3602" s="3"/>
+      <c r="E3602" s="4"/>
       <c r="F3602" s="1" t="s">
         <v>71</v>
       </c>
@@ -77569,10 +77582,10 @@
       <c r="C3603" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3603" s="3" t="s">
+      <c r="D3603" s="4" t="s">
         <v>804</v>
       </c>
-      <c r="E3603" s="3"/>
+      <c r="E3603" s="4"/>
       <c r="F3603" s="1" t="s">
         <v>71</v>
       </c>
@@ -77590,10 +77603,10 @@
       <c r="C3604" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3604" s="3" t="s">
+      <c r="D3604" s="4" t="s">
         <v>805</v>
       </c>
-      <c r="E3604" s="3"/>
+      <c r="E3604" s="4"/>
       <c r="F3604" s="1" t="s">
         <v>81</v>
       </c>
@@ -77611,10 +77624,10 @@
       <c r="C3605" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3605" s="3" t="s">
+      <c r="D3605" s="4" t="s">
         <v>806</v>
       </c>
-      <c r="E3605" s="3"/>
+      <c r="E3605" s="4"/>
       <c r="F3605" s="1" t="s">
         <v>85</v>
       </c>
@@ -77632,10 +77645,10 @@
       <c r="C3606" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3606" s="3" t="s">
+      <c r="D3606" s="4" t="s">
         <v>807</v>
       </c>
-      <c r="E3606" s="3"/>
+      <c r="E3606" s="4"/>
       <c r="F3606" s="1" t="s">
         <v>71</v>
       </c>
@@ -77644,10 +77657,10 @@
       </c>
     </row>
     <row r="3607" spans="1:7" ht="14.25" customHeight="1">
-      <c r="D3607" s="3" t="s">
+      <c r="D3607" s="4" t="s">
         <v>749</v>
       </c>
-      <c r="E3607" s="3"/>
+      <c r="E3607" s="4"/>
     </row>
     <row r="3608" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3608" s="2">
@@ -77659,10 +77672,10 @@
       <c r="C3608" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3608" s="3" t="s">
+      <c r="D3608" s="4" t="s">
         <v>808</v>
       </c>
-      <c r="E3608" s="3"/>
+      <c r="E3608" s="4"/>
       <c r="F3608" s="1" t="s">
         <v>71</v>
       </c>
@@ -77680,10 +77693,10 @@
       <c r="C3609" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3609" s="3" t="s">
+      <c r="D3609" s="4" t="s">
         <v>809</v>
       </c>
-      <c r="E3609" s="3"/>
+      <c r="E3609" s="4"/>
       <c r="F3609" s="1" t="s">
         <v>71</v>
       </c>
@@ -77701,10 +77714,10 @@
       <c r="C3610" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3610" s="3" t="s">
+      <c r="D3610" s="4" t="s">
         <v>810</v>
       </c>
-      <c r="E3610" s="3"/>
+      <c r="E3610" s="4"/>
       <c r="F3610" s="1" t="s">
         <v>81</v>
       </c>
@@ -78785,10 +78798,10 @@
       <c r="D3688" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="E3688" s="3" t="s">
+      <c r="E3688" s="4" t="s">
         <v>858</v>
       </c>
-      <c r="F3688" s="3"/>
+      <c r="F3688" s="4"/>
     </row>
     <row r="3689" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3689" s="2">
@@ -78803,10 +78816,10 @@
       <c r="D3689" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="E3689" s="3" t="s">
+      <c r="E3689" s="4" t="s">
         <v>859</v>
       </c>
-      <c r="F3689" s="3"/>
+      <c r="F3689" s="4"/>
     </row>
     <row r="3690" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3690" s="2">
@@ -78974,10 +78987,10 @@
       <c r="D3699" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="E3699" s="3" t="s">
+      <c r="E3699" s="4" t="s">
         <v>869</v>
       </c>
-      <c r="F3699" s="3"/>
+      <c r="F3699" s="4"/>
     </row>
     <row r="3700" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3700" s="2">
@@ -79201,7 +79214,7 @@
       </c>
     </row>
     <row r="3713" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A3713" s="4">
+      <c r="A3713" s="3">
         <v>10452</v>
       </c>
       <c r="B3713" s="1" t="s">
@@ -79434,10 +79447,10 @@
       <c r="D3726" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="E3726" s="3" t="s">
+      <c r="E3726" s="4" t="s">
         <v>890</v>
       </c>
-      <c r="F3726" s="3"/>
+      <c r="F3726" s="4"/>
     </row>
     <row r="3727" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3727" s="2">
@@ -79452,10 +79465,10 @@
       <c r="D3727" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="E3727" s="3" t="s">
+      <c r="E3727" s="4" t="s">
         <v>891</v>
       </c>
-      <c r="F3727" s="3"/>
+      <c r="F3727" s="4"/>
     </row>
     <row r="3728" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3728" s="2">
@@ -80167,10 +80180,10 @@
       <c r="D3769" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="E3769" s="3" t="s">
+      <c r="E3769" s="4" t="s">
         <v>929</v>
       </c>
-      <c r="F3769" s="3"/>
+      <c r="F3769" s="4"/>
     </row>
     <row r="3770" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3770" s="2">
@@ -80236,10 +80249,10 @@
       <c r="D3773" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="E3773" s="3" t="s">
+      <c r="E3773" s="4" t="s">
         <v>933</v>
       </c>
-      <c r="F3773" s="3"/>
+      <c r="F3773" s="4"/>
     </row>
     <row r="3774" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3774" s="2">
@@ -80254,10 +80267,10 @@
       <c r="D3774" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="E3774" s="3" t="s">
+      <c r="E3774" s="4" t="s">
         <v>934</v>
       </c>
-      <c r="F3774" s="3"/>
+      <c r="F3774" s="4"/>
     </row>
     <row r="3775" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3775" s="2">
@@ -80272,10 +80285,10 @@
       <c r="D3775" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="E3775" s="3" t="s">
+      <c r="E3775" s="4" t="s">
         <v>935</v>
       </c>
-      <c r="F3775" s="3"/>
+      <c r="F3775" s="4"/>
     </row>
     <row r="3776" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3776" s="2">
@@ -80290,10 +80303,10 @@
       <c r="D3776" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="E3776" s="3" t="s">
+      <c r="E3776" s="4" t="s">
         <v>936</v>
       </c>
-      <c r="F3776" s="3"/>
+      <c r="F3776" s="4"/>
     </row>
     <row r="3777" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3777" s="2">
@@ -80308,10 +80321,10 @@
       <c r="D3777" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="E3777" s="3" t="s">
+      <c r="E3777" s="4" t="s">
         <v>937</v>
       </c>
-      <c r="F3777" s="3"/>
+      <c r="F3777" s="4"/>
     </row>
     <row r="3778" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3778" s="2">
@@ -80445,10 +80458,10 @@
       <c r="D3785" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="E3785" s="3" t="s">
+      <c r="E3785" s="4" t="s">
         <v>945</v>
       </c>
-      <c r="F3785" s="3"/>
+      <c r="F3785" s="4"/>
     </row>
     <row r="3786" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3786" s="2">
@@ -80463,10 +80476,10 @@
       <c r="D3786" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="E3786" s="3" t="s">
+      <c r="E3786" s="4" t="s">
         <v>946</v>
       </c>
-      <c r="F3786" s="3"/>
+      <c r="F3786" s="4"/>
     </row>
     <row r="3787" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3787" s="2">
@@ -80634,10 +80647,10 @@
       <c r="D3796" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="E3796" s="3" t="s">
+      <c r="E3796" s="4" t="s">
         <v>956</v>
       </c>
-      <c r="F3796" s="3"/>
+      <c r="F3796" s="4"/>
     </row>
     <row r="3797" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3797" s="2">
@@ -84085,7 +84098,7 @@
       </c>
       <c r="G3958" s="2"/>
     </row>
-    <row r="3959" spans="1:7" ht="28">
+    <row r="3959" spans="1:7" ht="30">
       <c r="A3959" s="1">
         <v>10711</v>
       </c>
@@ -85887,15 +85900,132 @@
     <row r="4044" spans="1:11" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="159">
-    <mergeCell ref="E3777:F3777"/>
-    <mergeCell ref="E3776:F3776"/>
-    <mergeCell ref="E3775:F3775"/>
-    <mergeCell ref="E3774:F3774"/>
-    <mergeCell ref="E3773:F3773"/>
-    <mergeCell ref="E3769:F3769"/>
-    <mergeCell ref="E3727:F3727"/>
-    <mergeCell ref="E3726:F3726"/>
-    <mergeCell ref="E3785:F3785"/>
+    <mergeCell ref="E722:F722"/>
+    <mergeCell ref="E726:F726"/>
+    <mergeCell ref="E667:F667"/>
+    <mergeCell ref="E163:F163"/>
+    <mergeCell ref="E164:F164"/>
+    <mergeCell ref="B175:C175"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D3464:E3464"/>
+    <mergeCell ref="D3465:E3465"/>
+    <mergeCell ref="D3466:E3466"/>
+    <mergeCell ref="D3467:E3467"/>
+    <mergeCell ref="D3468:E3468"/>
+    <mergeCell ref="C3399:D3399"/>
+    <mergeCell ref="E3399:F3399"/>
+    <mergeCell ref="C3400:D3400"/>
+    <mergeCell ref="E3400:F3400"/>
+    <mergeCell ref="D3469:E3469"/>
+    <mergeCell ref="D3470:E3470"/>
+    <mergeCell ref="D3471:E3471"/>
+    <mergeCell ref="D3472:E3472"/>
+    <mergeCell ref="D3473:E3473"/>
+    <mergeCell ref="D3474:E3474"/>
+    <mergeCell ref="D3475:E3475"/>
+    <mergeCell ref="D3476:E3476"/>
+    <mergeCell ref="D3477:E3477"/>
+    <mergeCell ref="D3486:E3486"/>
+    <mergeCell ref="D3478:E3478"/>
+    <mergeCell ref="D3479:E3479"/>
+    <mergeCell ref="D3480:E3480"/>
+    <mergeCell ref="D3481:E3481"/>
+    <mergeCell ref="D3482:E3482"/>
+    <mergeCell ref="D3483:E3483"/>
+    <mergeCell ref="D3484:E3484"/>
+    <mergeCell ref="B3485:C3485"/>
+    <mergeCell ref="D3485:E3485"/>
+    <mergeCell ref="B3508:C3508"/>
+    <mergeCell ref="B3509:C3509"/>
+    <mergeCell ref="B3510:C3510"/>
+    <mergeCell ref="B3511:C3511"/>
+    <mergeCell ref="B3512:C3512"/>
+    <mergeCell ref="E3491:F3491"/>
+    <mergeCell ref="E3492:F3492"/>
+    <mergeCell ref="E3493:F3493"/>
+    <mergeCell ref="E3494:F3494"/>
+    <mergeCell ref="E3495:F3495"/>
+    <mergeCell ref="E3496:F3496"/>
+    <mergeCell ref="E3497:F3497"/>
+    <mergeCell ref="E3498:F3498"/>
+    <mergeCell ref="B3507:C3507"/>
+    <mergeCell ref="E3507:F3507"/>
+    <mergeCell ref="E3526:F3526"/>
+    <mergeCell ref="E3527:F3527"/>
+    <mergeCell ref="E3528:F3528"/>
+    <mergeCell ref="E3529:F3529"/>
+    <mergeCell ref="E3530:F3530"/>
+    <mergeCell ref="D3549:E3549"/>
+    <mergeCell ref="B3518:C3518"/>
+    <mergeCell ref="B3513:C3513"/>
+    <mergeCell ref="B3514:C3514"/>
+    <mergeCell ref="B3515:C3515"/>
+    <mergeCell ref="B3516:C3516"/>
+    <mergeCell ref="B3517:C3517"/>
+    <mergeCell ref="D3550:E3550"/>
+    <mergeCell ref="D3551:E3551"/>
+    <mergeCell ref="D3552:E3552"/>
+    <mergeCell ref="D3553:E3553"/>
+    <mergeCell ref="D3554:E3554"/>
+    <mergeCell ref="D3555:E3555"/>
+    <mergeCell ref="D3556:E3556"/>
+    <mergeCell ref="D3557:E3557"/>
+    <mergeCell ref="D3558:E3558"/>
+    <mergeCell ref="D3559:E3559"/>
+    <mergeCell ref="D3560:E3560"/>
+    <mergeCell ref="D3561:E3561"/>
+    <mergeCell ref="D3562:E3562"/>
+    <mergeCell ref="D3563:E3563"/>
+    <mergeCell ref="D3564:E3564"/>
+    <mergeCell ref="D3565:E3565"/>
+    <mergeCell ref="D3566:E3566"/>
+    <mergeCell ref="D3567:E3567"/>
+    <mergeCell ref="D3568:E3568"/>
+    <mergeCell ref="D3569:E3569"/>
+    <mergeCell ref="D3570:E3570"/>
+    <mergeCell ref="D3571:E3571"/>
+    <mergeCell ref="D3572:E3572"/>
+    <mergeCell ref="D3573:E3573"/>
+    <mergeCell ref="D3574:E3574"/>
+    <mergeCell ref="D3575:E3575"/>
+    <mergeCell ref="D3576:E3576"/>
+    <mergeCell ref="D3577:E3577"/>
+    <mergeCell ref="D3578:E3578"/>
+    <mergeCell ref="D3579:E3579"/>
+    <mergeCell ref="D3580:E3580"/>
+    <mergeCell ref="D3581:E3581"/>
+    <mergeCell ref="D3582:E3582"/>
+    <mergeCell ref="D3583:E3583"/>
+    <mergeCell ref="D3584:E3584"/>
+    <mergeCell ref="D3585:E3585"/>
+    <mergeCell ref="D3603:E3603"/>
+    <mergeCell ref="D3586:E3586"/>
+    <mergeCell ref="D3587:E3587"/>
+    <mergeCell ref="D3588:E3588"/>
+    <mergeCell ref="D3589:E3589"/>
+    <mergeCell ref="D3590:E3590"/>
+    <mergeCell ref="D3591:E3591"/>
+    <mergeCell ref="D3592:E3592"/>
+    <mergeCell ref="D3593:E3593"/>
+    <mergeCell ref="D3594:E3594"/>
+    <mergeCell ref="E3512:F3512"/>
+    <mergeCell ref="E3511:F3511"/>
+    <mergeCell ref="E3510:F3510"/>
+    <mergeCell ref="E3509:F3509"/>
+    <mergeCell ref="E3508:F3508"/>
+    <mergeCell ref="E3490:F3490"/>
+    <mergeCell ref="E3489:F3489"/>
+    <mergeCell ref="E3488:F3488"/>
+    <mergeCell ref="E3487:F3487"/>
+    <mergeCell ref="E3521:F3521"/>
+    <mergeCell ref="E3520:F3520"/>
+    <mergeCell ref="E3519:F3519"/>
+    <mergeCell ref="E3518:F3518"/>
+    <mergeCell ref="E3517:F3517"/>
+    <mergeCell ref="E3516:F3516"/>
+    <mergeCell ref="E3515:F3515"/>
+    <mergeCell ref="E3514:F3514"/>
+    <mergeCell ref="E3513:F3513"/>
     <mergeCell ref="E3786:F3786"/>
     <mergeCell ref="E3796:F3796"/>
     <mergeCell ref="E3688:F3688"/>
@@ -85905,24 +86035,6 @@
     <mergeCell ref="E3524:F3524"/>
     <mergeCell ref="E3523:F3523"/>
     <mergeCell ref="E3522:F3522"/>
-    <mergeCell ref="E3521:F3521"/>
-    <mergeCell ref="E3520:F3520"/>
-    <mergeCell ref="E3519:F3519"/>
-    <mergeCell ref="E3518:F3518"/>
-    <mergeCell ref="E3517:F3517"/>
-    <mergeCell ref="E3516:F3516"/>
-    <mergeCell ref="E3515:F3515"/>
-    <mergeCell ref="E3514:F3514"/>
-    <mergeCell ref="E3513:F3513"/>
-    <mergeCell ref="E3512:F3512"/>
-    <mergeCell ref="E3511:F3511"/>
-    <mergeCell ref="E3510:F3510"/>
-    <mergeCell ref="E3509:F3509"/>
-    <mergeCell ref="E3508:F3508"/>
-    <mergeCell ref="E3490:F3490"/>
-    <mergeCell ref="E3489:F3489"/>
-    <mergeCell ref="E3488:F3488"/>
-    <mergeCell ref="E3487:F3487"/>
     <mergeCell ref="D3604:E3604"/>
     <mergeCell ref="D3605:E3605"/>
     <mergeCell ref="D3606:E3606"/>
@@ -85938,114 +86050,15 @@
     <mergeCell ref="D3600:E3600"/>
     <mergeCell ref="D3601:E3601"/>
     <mergeCell ref="D3602:E3602"/>
-    <mergeCell ref="D3603:E3603"/>
-    <mergeCell ref="D3586:E3586"/>
-    <mergeCell ref="D3587:E3587"/>
-    <mergeCell ref="D3588:E3588"/>
-    <mergeCell ref="D3589:E3589"/>
-    <mergeCell ref="D3590:E3590"/>
-    <mergeCell ref="D3591:E3591"/>
-    <mergeCell ref="D3592:E3592"/>
-    <mergeCell ref="D3593:E3593"/>
-    <mergeCell ref="D3594:E3594"/>
-    <mergeCell ref="D3577:E3577"/>
-    <mergeCell ref="D3578:E3578"/>
-    <mergeCell ref="D3579:E3579"/>
-    <mergeCell ref="D3580:E3580"/>
-    <mergeCell ref="D3581:E3581"/>
-    <mergeCell ref="D3582:E3582"/>
-    <mergeCell ref="D3583:E3583"/>
-    <mergeCell ref="D3584:E3584"/>
-    <mergeCell ref="D3585:E3585"/>
-    <mergeCell ref="D3568:E3568"/>
-    <mergeCell ref="D3569:E3569"/>
-    <mergeCell ref="D3570:E3570"/>
-    <mergeCell ref="D3571:E3571"/>
-    <mergeCell ref="D3572:E3572"/>
-    <mergeCell ref="D3573:E3573"/>
-    <mergeCell ref="D3574:E3574"/>
-    <mergeCell ref="D3575:E3575"/>
-    <mergeCell ref="D3576:E3576"/>
-    <mergeCell ref="D3559:E3559"/>
-    <mergeCell ref="D3560:E3560"/>
-    <mergeCell ref="D3561:E3561"/>
-    <mergeCell ref="D3562:E3562"/>
-    <mergeCell ref="D3563:E3563"/>
-    <mergeCell ref="D3564:E3564"/>
-    <mergeCell ref="D3565:E3565"/>
-    <mergeCell ref="D3566:E3566"/>
-    <mergeCell ref="D3567:E3567"/>
-    <mergeCell ref="D3550:E3550"/>
-    <mergeCell ref="D3551:E3551"/>
-    <mergeCell ref="D3552:E3552"/>
-    <mergeCell ref="D3553:E3553"/>
-    <mergeCell ref="D3554:E3554"/>
-    <mergeCell ref="D3555:E3555"/>
-    <mergeCell ref="D3556:E3556"/>
-    <mergeCell ref="D3557:E3557"/>
-    <mergeCell ref="D3558:E3558"/>
-    <mergeCell ref="E3526:F3526"/>
-    <mergeCell ref="E3527:F3527"/>
-    <mergeCell ref="E3528:F3528"/>
-    <mergeCell ref="E3529:F3529"/>
-    <mergeCell ref="E3530:F3530"/>
-    <mergeCell ref="D3549:E3549"/>
-    <mergeCell ref="B3518:C3518"/>
-    <mergeCell ref="B3513:C3513"/>
-    <mergeCell ref="B3514:C3514"/>
-    <mergeCell ref="B3515:C3515"/>
-    <mergeCell ref="B3516:C3516"/>
-    <mergeCell ref="B3517:C3517"/>
-    <mergeCell ref="B3508:C3508"/>
-    <mergeCell ref="B3509:C3509"/>
-    <mergeCell ref="B3510:C3510"/>
-    <mergeCell ref="B3511:C3511"/>
-    <mergeCell ref="B3512:C3512"/>
-    <mergeCell ref="E3491:F3491"/>
-    <mergeCell ref="E3492:F3492"/>
-    <mergeCell ref="E3493:F3493"/>
-    <mergeCell ref="E3494:F3494"/>
-    <mergeCell ref="E3495:F3495"/>
-    <mergeCell ref="E3496:F3496"/>
-    <mergeCell ref="E3497:F3497"/>
-    <mergeCell ref="E3498:F3498"/>
-    <mergeCell ref="B3507:C3507"/>
-    <mergeCell ref="E3507:F3507"/>
-    <mergeCell ref="D3486:E3486"/>
-    <mergeCell ref="D3478:E3478"/>
-    <mergeCell ref="D3479:E3479"/>
-    <mergeCell ref="D3480:E3480"/>
-    <mergeCell ref="D3481:E3481"/>
-    <mergeCell ref="D3482:E3482"/>
-    <mergeCell ref="D3483:E3483"/>
-    <mergeCell ref="D3484:E3484"/>
-    <mergeCell ref="B3485:C3485"/>
-    <mergeCell ref="D3485:E3485"/>
-    <mergeCell ref="D3469:E3469"/>
-    <mergeCell ref="D3470:E3470"/>
-    <mergeCell ref="D3471:E3471"/>
-    <mergeCell ref="D3472:E3472"/>
-    <mergeCell ref="D3473:E3473"/>
-    <mergeCell ref="D3474:E3474"/>
-    <mergeCell ref="D3475:E3475"/>
-    <mergeCell ref="D3476:E3476"/>
-    <mergeCell ref="D3477:E3477"/>
-    <mergeCell ref="D3464:E3464"/>
-    <mergeCell ref="D3465:E3465"/>
-    <mergeCell ref="D3466:E3466"/>
-    <mergeCell ref="D3467:E3467"/>
-    <mergeCell ref="D3468:E3468"/>
-    <mergeCell ref="C3399:D3399"/>
-    <mergeCell ref="E3399:F3399"/>
-    <mergeCell ref="C3400:D3400"/>
-    <mergeCell ref="E3400:F3400"/>
-    <mergeCell ref="E722:F722"/>
-    <mergeCell ref="E726:F726"/>
-    <mergeCell ref="E667:F667"/>
-    <mergeCell ref="E163:F163"/>
-    <mergeCell ref="E164:F164"/>
-    <mergeCell ref="B175:C175"/>
-    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E3777:F3777"/>
+    <mergeCell ref="E3776:F3776"/>
+    <mergeCell ref="E3775:F3775"/>
+    <mergeCell ref="E3774:F3774"/>
+    <mergeCell ref="E3773:F3773"/>
+    <mergeCell ref="E3769:F3769"/>
+    <mergeCell ref="E3727:F3727"/>
+    <mergeCell ref="E3726:F3726"/>
+    <mergeCell ref="E3785:F3785"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>